<commit_message>
metric support on friction loss
</commit_message>
<xml_diff>
--- a/kb/unit-converter/volume.xlsx
+++ b/kb/unit-converter/volume.xlsx
@@ -106,7 +106,7 @@
     <t xml:space="preserve">USgallons</t>
   </si>
   <si>
-    <t xml:space="preserve">barrels</t>
+    <t xml:space="preserve">barrels (oil)</t>
   </si>
   <si>
     <t xml:space="preserve">liter</t>
@@ -137,7 +137,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -173,11 +173,6 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -252,7 +247,7 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -336,7 +331,7 @@
   <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
+      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>